<commit_message>
1.add a case in ROL_Functional_Test_Matrix.json and add sleep time (60s) after run the first case 2.remove "msg.setField(fix.HandlInst('1'))"
</commit_message>
<xml_diff>
--- a/rolx_fix_client/initiator/rolx_regression_test/report/rolx_report.xlsx
+++ b/rolx_fix_client/initiator/rolx_regression_test/report/rolx_report.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,7 +563,7 @@
     <row r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>63</t>
         </is>
       </c>
       <c r="B2" s="4" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="I2" s="4" t="inlineStr">
         <is>
-          <t>5110</t>
+          <t>1301</t>
         </is>
       </c>
       <c r="J2" s="4" t="inlineStr">
@@ -630,13 +630,21 @@
         </is>
       </c>
       <c r="O2" s="4" t="inlineStr"/>
-      <c r="P2" s="4" t="n"/>
-      <c r="Q2" s="4" t="n"/>
+      <c r="P2" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="Q2" s="4" t="inlineStr">
+        <is>
+          <t>ps: 若列表存在failed数据，请查看report.log文件</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" s="4" t="inlineStr">
@@ -669,7 +677,7 @@
       </c>
       <c r="H3" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I3" s="4" t="inlineStr">
@@ -703,13 +711,21 @@
         </is>
       </c>
       <c r="O3" s="4" t="inlineStr"/>
-      <c r="P3" s="4" t="n"/>
-      <c r="Q3" s="4" t="n"/>
+      <c r="P3" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="Q3" s="4" t="inlineStr">
+        <is>
+          <t>Market Price is OK</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B4" s="4" t="inlineStr">
@@ -729,7 +745,7 @@
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Limit_NewAck</t>
+          <t>ROLX_Market_NewAck</t>
         </is>
       </c>
       <c r="F4" s="4" t="n">
@@ -737,12 +753,12 @@
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H4" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I4" s="4" t="inlineStr">
@@ -775,16 +791,22 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O4" s="4" t="n">
-        <v>1230</v>
-      </c>
-      <c r="P4" s="4" t="n"/>
-      <c r="Q4" s="4" t="n"/>
+      <c r="O4" s="4" t="inlineStr"/>
+      <c r="P4" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="Q4" s="4" t="inlineStr">
+        <is>
+          <t>FixMsg is OK</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
@@ -817,7 +839,7 @@
       </c>
       <c r="H5" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I5" s="4" t="inlineStr">
@@ -853,18 +875,22 @@
       <c r="O5" s="4" t="n">
         <v>1230</v>
       </c>
-      <c r="P5" s="4" t="n"/>
+      <c r="P5" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q5" s="4" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>New Order-&gt;Partial Fill-&gt;Fill</t>
+          <t>New Order-&gt;Fill</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -879,7 +905,7 @@
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Market_NewAck</t>
+          <t>ROLX_Limit_NewAck</t>
         </is>
       </c>
       <c r="F6" s="4" t="n">
@@ -887,17 +913,17 @@
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H6" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I6" s="4" t="inlineStr">
         <is>
-          <t>6028</t>
+          <t>5110</t>
         </is>
       </c>
       <c r="J6" s="4" t="inlineStr">
@@ -925,14 +951,20 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O6" s="4" t="inlineStr"/>
-      <c r="P6" s="4" t="n"/>
+      <c r="O6" s="4" t="n">
+        <v>1230</v>
+      </c>
+      <c r="P6" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q6" s="4" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B7" s="4" t="inlineStr">
@@ -952,7 +984,7 @@
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Limit_NewAck</t>
+          <t>ROLX_Market_NewAck</t>
         </is>
       </c>
       <c r="F7" s="4" t="n">
@@ -965,7 +997,7 @@
       </c>
       <c r="H7" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I7" s="4" t="inlineStr">
@@ -999,13 +1031,17 @@
         </is>
       </c>
       <c r="O7" s="4" t="inlineStr"/>
-      <c r="P7" s="4" t="n"/>
+      <c r="P7" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q7" s="4" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B8" s="4" t="inlineStr">
@@ -1033,12 +1069,12 @@
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H8" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I8" s="4" t="inlineStr">
@@ -1071,16 +1107,22 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O8" s="4" t="n">
-        <v>3470</v>
-      </c>
-      <c r="P8" s="4" t="n"/>
-      <c r="Q8" s="4" t="n"/>
+      <c r="O8" s="4" t="inlineStr"/>
+      <c r="P8" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="Q8" s="4" t="inlineStr">
+        <is>
+          <t>execType is OK</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B9" s="4" t="inlineStr">
@@ -1113,7 +1155,7 @@
       </c>
       <c r="H9" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I9" s="4" t="inlineStr">
@@ -1149,18 +1191,22 @@
       <c r="O9" s="4" t="n">
         <v>3470</v>
       </c>
-      <c r="P9" s="4" t="n"/>
+      <c r="P9" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q9" s="4" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>New Order-&gt;Partial Fill-&gt;Canceled</t>
+          <t>New Order-&gt;Partial Fill-&gt;Fill</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
@@ -1175,7 +1221,7 @@
       </c>
       <c r="E10" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Market_NewAck</t>
+          <t>ROLX_Limit_NewAck</t>
         </is>
       </c>
       <c r="F10" s="4" t="n">
@@ -1183,17 +1229,17 @@
       </c>
       <c r="G10" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H10" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I10" s="4" t="inlineStr">
         <is>
-          <t>5076</t>
+          <t>6028</t>
         </is>
       </c>
       <c r="J10" s="4" t="inlineStr">
@@ -1221,19 +1267,25 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O10" s="4" t="inlineStr"/>
-      <c r="P10" s="4" t="n"/>
+      <c r="O10" s="4" t="n">
+        <v>3470</v>
+      </c>
+      <c r="P10" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q10" s="4" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>Canceled</t>
+          <t>New Order-&gt;Partial Fill-&gt;Canceled</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
@@ -1243,12 +1295,12 @@
       </c>
       <c r="D11" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>NewAck</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>ROLX_Market_NewAck</t>
         </is>
       </c>
       <c r="F11" s="4" t="n">
@@ -1295,18 +1347,22 @@
         </is>
       </c>
       <c r="O11" s="4" t="inlineStr"/>
-      <c r="P11" s="4" t="n"/>
+      <c r="P11" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q11" s="4" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>New Order-&gt;Partial Fill-&gt;Canceled</t>
+          <t>Canceled</t>
         </is>
       </c>
       <c r="C12" s="4" t="inlineStr">
@@ -1316,12 +1372,12 @@
       </c>
       <c r="D12" s="4" t="inlineStr">
         <is>
-          <t>NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="E12" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Limit_NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="F12" s="4" t="n">
@@ -1329,12 +1385,12 @@
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H12" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I12" s="4" t="inlineStr">
@@ -1367,21 +1423,23 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O12" s="4" t="n">
-        <v>1037</v>
-      </c>
-      <c r="P12" s="4" t="n"/>
+      <c r="O12" s="4" t="inlineStr"/>
+      <c r="P12" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q12" s="4" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>Canceled</t>
+          <t>New Order-&gt;Partial Fill-&gt;Canceled</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
@@ -1391,12 +1449,12 @@
       </c>
       <c r="D13" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>NewAck</t>
         </is>
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>ROLX_Limit_NewAck</t>
         </is>
       </c>
       <c r="F13" s="4" t="n">
@@ -1442,19 +1500,25 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O13" s="4" t="inlineStr"/>
-      <c r="P13" s="4" t="n"/>
+      <c r="O13" s="4" t="n">
+        <v>1037</v>
+      </c>
+      <c r="P13" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q13" s="4" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>New Order-&gt;Partial Fill-&gt;Expired</t>
+          <t>Canceled</t>
         </is>
       </c>
       <c r="C14" s="4" t="inlineStr">
@@ -1464,12 +1528,12 @@
       </c>
       <c r="D14" s="4" t="inlineStr">
         <is>
-          <t>NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="E14" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Market_NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="F14" s="4" t="n">
@@ -1477,17 +1541,17 @@
       </c>
       <c r="G14" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H14" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I14" s="4" t="inlineStr">
         <is>
-          <t>5108</t>
+          <t>5076</t>
         </is>
       </c>
       <c r="J14" s="4" t="inlineStr">
@@ -1516,13 +1580,17 @@
         </is>
       </c>
       <c r="O14" s="4" t="inlineStr"/>
-      <c r="P14" s="4" t="n"/>
+      <c r="P14" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q14" s="4" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
@@ -1542,7 +1610,7 @@
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Limit_NewAck</t>
+          <t>ROLX_Market_NewAck</t>
         </is>
       </c>
       <c r="F15" s="4" t="n">
@@ -1550,12 +1618,12 @@
       </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H15" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I15" s="4" t="inlineStr">
@@ -1588,21 +1656,23 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O15" s="4" t="n">
-        <v>5222</v>
-      </c>
-      <c r="P15" s="4" t="n"/>
+      <c r="O15" s="4" t="inlineStr"/>
+      <c r="P15" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q15" s="4" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>New Order-&gt;Canceled</t>
+          <t>New Order-&gt;Partial Fill-&gt;Expired</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
@@ -1617,7 +1687,7 @@
       </c>
       <c r="E16" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Market_NewAck</t>
+          <t>ROLX_Limit_NewAck</t>
         </is>
       </c>
       <c r="F16" s="4" t="n">
@@ -1625,17 +1695,17 @@
       </c>
       <c r="G16" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H16" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I16" s="4" t="inlineStr">
         <is>
-          <t>1311</t>
+          <t>5108</t>
         </is>
       </c>
       <c r="J16" s="4" t="inlineStr">
@@ -1663,14 +1733,20 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O16" s="4" t="inlineStr"/>
-      <c r="P16" s="4" t="n"/>
+      <c r="O16" s="4" t="n">
+        <v>5222</v>
+      </c>
+      <c r="P16" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q16" s="4" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
@@ -1685,12 +1761,12 @@
       </c>
       <c r="D17" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>NewAck</t>
         </is>
       </c>
       <c r="E17" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>ROLX_Market_NewAck</t>
         </is>
       </c>
       <c r="F17" s="4" t="n">
@@ -1737,13 +1813,17 @@
         </is>
       </c>
       <c r="O17" s="4" t="inlineStr"/>
-      <c r="P17" s="4" t="n"/>
+      <c r="P17" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q17" s="4" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
@@ -1758,12 +1838,12 @@
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
-          <t>NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="E18" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Market_NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="F18" s="4" t="n">
@@ -1776,7 +1856,7 @@
       </c>
       <c r="H18" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I18" s="4" t="inlineStr">
@@ -1810,13 +1890,17 @@
         </is>
       </c>
       <c r="O18" s="4" t="inlineStr"/>
-      <c r="P18" s="4" t="n"/>
+      <c r="P18" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q18" s="4" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>17</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
@@ -1831,12 +1915,12 @@
       </c>
       <c r="D19" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>NewAck</t>
         </is>
       </c>
       <c r="E19" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>ROLX_Market_NewAck</t>
         </is>
       </c>
       <c r="F19" s="4" t="n">
@@ -1883,13 +1967,17 @@
         </is>
       </c>
       <c r="O19" s="4" t="inlineStr"/>
-      <c r="P19" s="4" t="n"/>
+      <c r="P19" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q19" s="4" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>18</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
@@ -1904,12 +1992,12 @@
       </c>
       <c r="D20" s="4" t="inlineStr">
         <is>
-          <t>NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="E20" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Limit_NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="F20" s="4" t="n">
@@ -1917,12 +2005,12 @@
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H20" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I20" s="4" t="inlineStr">
@@ -1955,16 +2043,18 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O20" s="4" t="n">
-        <v>973</v>
-      </c>
-      <c r="P20" s="4" t="n"/>
+      <c r="O20" s="4" t="inlineStr"/>
+      <c r="P20" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q20" s="4" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>19</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
@@ -1979,12 +2069,12 @@
       </c>
       <c r="D21" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>NewAck</t>
         </is>
       </c>
       <c r="E21" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>ROLX_Limit_NewAck</t>
         </is>
       </c>
       <c r="F21" s="4" t="n">
@@ -2033,13 +2123,17 @@
       <c r="O21" s="4" t="n">
         <v>973</v>
       </c>
-      <c r="P21" s="4" t="n"/>
+      <c r="P21" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q21" s="4" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
@@ -2054,12 +2148,12 @@
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Limit_NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="F22" s="4" t="n">
@@ -2072,7 +2166,7 @@
       </c>
       <c r="H22" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
@@ -2108,13 +2202,17 @@
       <c r="O22" s="4" t="n">
         <v>973</v>
       </c>
-      <c r="P22" s="4" t="n"/>
+      <c r="P22" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q22" s="4" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
@@ -2129,12 +2227,12 @@
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>NewAck</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>ROLX_Limit_NewAck</t>
         </is>
       </c>
       <c r="F23" s="4" t="n">
@@ -2183,18 +2281,22 @@
       <c r="O23" s="4" t="n">
         <v>973</v>
       </c>
-      <c r="P23" s="4" t="n"/>
+      <c r="P23" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q23" s="4" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>New Order-&gt;Expired</t>
+          <t>New Order-&gt;Canceled</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
@@ -2204,12 +2306,12 @@
       </c>
       <c r="D24" s="4" t="inlineStr">
         <is>
-          <t>NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="E24" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Market_NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="F24" s="4" t="n">
@@ -2217,17 +2319,17 @@
       </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H24" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I24" s="4" t="inlineStr">
         <is>
-          <t>1313</t>
+          <t>1311</t>
         </is>
       </c>
       <c r="J24" s="4" t="inlineStr">
@@ -2255,14 +2357,20 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O24" s="4" t="inlineStr"/>
-      <c r="P24" s="4" t="n"/>
+      <c r="O24" s="4" t="n">
+        <v>973</v>
+      </c>
+      <c r="P24" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q24" s="4" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>23</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
@@ -2295,7 +2403,7 @@
       </c>
       <c r="H25" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -2329,13 +2437,17 @@
         </is>
       </c>
       <c r="O25" s="4" t="inlineStr"/>
-      <c r="P25" s="4" t="n"/>
+      <c r="P25" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q25" s="4" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>24</t>
         </is>
       </c>
       <c r="B26" s="4" t="inlineStr">
@@ -2355,7 +2467,7 @@
       </c>
       <c r="E26" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Limit_NewAck</t>
+          <t>ROLX_Market_NewAck</t>
         </is>
       </c>
       <c r="F26" s="4" t="n">
@@ -2363,12 +2475,12 @@
       </c>
       <c r="G26" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H26" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I26" s="4" t="inlineStr">
@@ -2401,16 +2513,18 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O26" s="4" t="n">
-        <v>3365</v>
-      </c>
-      <c r="P26" s="4" t="n"/>
+      <c r="O26" s="4" t="inlineStr"/>
+      <c r="P26" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q26" s="4" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>25</t>
         </is>
       </c>
       <c r="B27" s="4" t="inlineStr">
@@ -2443,7 +2557,7 @@
       </c>
       <c r="H27" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I27" s="4" t="inlineStr">
@@ -2479,18 +2593,22 @@
       <c r="O27" s="4" t="n">
         <v>3365</v>
       </c>
-      <c r="P27" s="4" t="n"/>
+      <c r="P27" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q27" s="4" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>BBO Price Rounding Check</t>
+          <t>New Order-&gt;Expired</t>
         </is>
       </c>
       <c r="C28" s="4" t="inlineStr">
@@ -2505,7 +2623,7 @@
       </c>
       <c r="E28" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Market_NewAck</t>
+          <t>ROLX_Limit_NewAck</t>
         </is>
       </c>
       <c r="F28" s="4" t="n">
@@ -2513,17 +2631,17 @@
       </c>
       <c r="G28" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H28" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I28" s="4" t="inlineStr">
         <is>
-          <t>4689</t>
+          <t>1313</t>
         </is>
       </c>
       <c r="J28" s="4" t="inlineStr">
@@ -2551,14 +2669,20 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O28" s="4" t="inlineStr"/>
-      <c r="P28" s="4" t="n"/>
+      <c r="O28" s="4" t="n">
+        <v>3365</v>
+      </c>
+      <c r="P28" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q28" s="4" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>27</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
@@ -2591,7 +2715,7 @@
       </c>
       <c r="H29" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I29" s="4" t="inlineStr">
@@ -2625,13 +2749,17 @@
         </is>
       </c>
       <c r="O29" s="4" t="inlineStr"/>
-      <c r="P29" s="4" t="n"/>
+      <c r="P29" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q29" s="4" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B30" s="4" t="inlineStr">
@@ -2651,7 +2779,7 @@
       </c>
       <c r="E30" s="4" t="inlineStr">
         <is>
-          <t>ROLX_Limit_NewAck</t>
+          <t>ROLX_Market_NewAck</t>
         </is>
       </c>
       <c r="F30" s="4" t="n">
@@ -2659,12 +2787,12 @@
       </c>
       <c r="G30" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H30" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I30" s="4" t="inlineStr">
@@ -2697,16 +2825,18 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O30" s="4" t="n">
-        <v>369</v>
-      </c>
-      <c r="P30" s="4" t="n"/>
+      <c r="O30" s="4" t="inlineStr"/>
+      <c r="P30" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q30" s="4" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>29</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
@@ -2739,7 +2869,7 @@
       </c>
       <c r="H31" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I31" s="4" t="inlineStr">
@@ -2775,18 +2905,22 @@
       <c r="O31" s="4" t="n">
         <v>369</v>
       </c>
-      <c r="P31" s="4" t="n"/>
+      <c r="P31" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q31" s="4" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>30</t>
         </is>
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>Symbol Check</t>
+          <t>BBO Price Rounding Check</t>
         </is>
       </c>
       <c r="C32" s="4" t="inlineStr">
@@ -2819,7 +2953,7 @@
       </c>
       <c r="I32" s="4" t="inlineStr">
         <is>
-          <t>9999</t>
+          <t>4689</t>
         </is>
       </c>
       <c r="J32" s="4" t="inlineStr">
@@ -2850,18 +2984,22 @@
       <c r="O32" s="4" t="n">
         <v>369</v>
       </c>
-      <c r="P32" s="4" t="n"/>
+      <c r="P32" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q32" s="4" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>31</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Price Limit Check</t>
+          <t>Symbol Check</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
@@ -2876,7 +3014,7 @@
       </c>
       <c r="E33" s="4" t="inlineStr">
         <is>
-          <t>Price=Low-limit-1</t>
+          <t>ROLX_Limit_NewAck</t>
         </is>
       </c>
       <c r="F33" s="4" t="n">
@@ -2894,7 +3032,7 @@
       </c>
       <c r="I33" s="4" t="inlineStr">
         <is>
-          <t>1324</t>
+          <t>9999</t>
         </is>
       </c>
       <c r="J33" s="4" t="inlineStr">
@@ -2923,15 +3061,19 @@
         </is>
       </c>
       <c r="O33" s="4" t="n">
-        <v>58</v>
-      </c>
-      <c r="P33" s="4" t="n"/>
+        <v>369</v>
+      </c>
+      <c r="P33" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q33" s="4" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr">
@@ -2951,7 +3093,7 @@
       </c>
       <c r="E34" s="4" t="inlineStr">
         <is>
-          <t>Price=High-limit+1</t>
+          <t>Price=Low-limit-1</t>
         </is>
       </c>
       <c r="F34" s="4" t="n">
@@ -2998,20 +3140,24 @@
         </is>
       </c>
       <c r="O34" s="4" t="n">
-        <v>119</v>
-      </c>
-      <c r="P34" s="4" t="n"/>
+        <v>58</v>
+      </c>
+      <c r="P34" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q34" s="4" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>Tick Size Check</t>
+          <t>Price Limit Check</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
@@ -3026,7 +3172,7 @@
       </c>
       <c r="E35" s="4" t="inlineStr">
         <is>
-          <t>Price&lt;1,000 Tick size ≠ 1</t>
+          <t>Price=High-limit+1</t>
         </is>
       </c>
       <c r="F35" s="4" t="n">
@@ -3044,7 +3190,7 @@
       </c>
       <c r="I35" s="4" t="inlineStr">
         <is>
-          <t>4689</t>
+          <t>1324</t>
         </is>
       </c>
       <c r="J35" s="4" t="inlineStr">
@@ -3073,15 +3219,19 @@
         </is>
       </c>
       <c r="O35" s="4" t="n">
-        <v>371.5</v>
-      </c>
-      <c r="P35" s="4" t="n"/>
+        <v>119</v>
+      </c>
+      <c r="P35" s="4" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
       <c r="Q35" s="4" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B36" s="4" t="inlineStr">
@@ -3101,7 +3251,7 @@
       </c>
       <c r="E36" s="4" t="inlineStr">
         <is>
-          <t>Price&lt;3,000 Tick side ≠ 1</t>
+          <t>Price&lt;1,000 Tick size ≠ 1</t>
         </is>
       </c>
       <c r="F36" s="4" t="n">
@@ -3119,7 +3269,7 @@
       </c>
       <c r="I36" s="4" t="inlineStr">
         <is>
-          <t>7203</t>
+          <t>4689</t>
         </is>
       </c>
       <c r="J36" s="4" t="inlineStr">
@@ -3148,7 +3298,7 @@
         </is>
       </c>
       <c r="O36" s="4" t="n">
-        <v>2105.5</v>
+        <v>371.5</v>
       </c>
       <c r="P36" s="4" t="n"/>
       <c r="Q36" s="4" t="n"/>
@@ -3156,7 +3306,7 @@
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>35</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
@@ -3176,7 +3326,7 @@
       </c>
       <c r="E37" s="4" t="inlineStr">
         <is>
-          <t>Price&lt;10,000 Tick side ≠ 1</t>
+          <t>Price&lt;3,000 Tick side ≠ 1</t>
         </is>
       </c>
       <c r="F37" s="4" t="n">
@@ -3194,7 +3344,7 @@
       </c>
       <c r="I37" s="4" t="inlineStr">
         <is>
-          <t>9433</t>
+          <t>7203</t>
         </is>
       </c>
       <c r="J37" s="4" t="inlineStr">
@@ -3223,7 +3373,7 @@
         </is>
       </c>
       <c r="O37" s="4" t="n">
-        <v>5000.5</v>
+        <v>2105.5</v>
       </c>
       <c r="P37" s="4" t="n"/>
       <c r="Q37" s="4" t="n"/>
@@ -3231,7 +3381,7 @@
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>36</t>
         </is>
       </c>
       <c r="B38" s="4" t="inlineStr">
@@ -3251,7 +3401,7 @@
       </c>
       <c r="E38" s="4" t="inlineStr">
         <is>
-          <t>Price&lt;30,000 Tick side ≠ 5</t>
+          <t>Price&lt;10,000 Tick side ≠ 1</t>
         </is>
       </c>
       <c r="F38" s="4" t="n">
@@ -3269,7 +3419,7 @@
       </c>
       <c r="I38" s="4" t="inlineStr">
         <is>
-          <t>6954</t>
+          <t>9433</t>
         </is>
       </c>
       <c r="J38" s="4" t="inlineStr">
@@ -3298,7 +3448,7 @@
         </is>
       </c>
       <c r="O38" s="4" t="n">
-        <v>26001</v>
+        <v>5000.5</v>
       </c>
       <c r="P38" s="4" t="n"/>
       <c r="Q38" s="4" t="n"/>
@@ -3306,7 +3456,7 @@
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr">
@@ -3326,7 +3476,7 @@
       </c>
       <c r="E39" s="4" t="inlineStr">
         <is>
-          <t>Price&lt;100,000 Tick side ≠ 10</t>
+          <t>Price&lt;30,000 Tick side ≠ 5</t>
         </is>
       </c>
       <c r="F39" s="4" t="n">
@@ -3344,7 +3494,7 @@
       </c>
       <c r="I39" s="4" t="inlineStr">
         <is>
-          <t>9983</t>
+          <t>6954</t>
         </is>
       </c>
       <c r="J39" s="4" t="inlineStr">
@@ -3373,7 +3523,7 @@
         </is>
       </c>
       <c r="O39" s="4" t="n">
-        <v>75001</v>
+        <v>26001</v>
       </c>
       <c r="P39" s="4" t="n"/>
       <c r="Q39" s="4" t="n"/>
@@ -3381,7 +3531,7 @@
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>38</t>
         </is>
       </c>
       <c r="B40" s="4" t="inlineStr">
@@ -3401,7 +3551,7 @@
       </c>
       <c r="E40" s="4" t="inlineStr">
         <is>
-          <t>Price&lt;3,000 Tick side ≠ 1</t>
+          <t>Price&lt;100,000 Tick side ≠ 10</t>
         </is>
       </c>
       <c r="F40" s="4" t="n">
@@ -3419,7 +3569,7 @@
       </c>
       <c r="I40" s="4" t="inlineStr">
         <is>
-          <t>1721</t>
+          <t>9983</t>
         </is>
       </c>
       <c r="J40" s="4" t="inlineStr">
@@ -3448,7 +3598,7 @@
         </is>
       </c>
       <c r="O40" s="4" t="n">
-        <v>2500.5</v>
+        <v>75001</v>
       </c>
       <c r="P40" s="4" t="n"/>
       <c r="Q40" s="4" t="n"/>
@@ -3456,7 +3606,7 @@
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
@@ -3476,7 +3626,7 @@
       </c>
       <c r="E41" s="4" t="inlineStr">
         <is>
-          <t>Price&lt;5,000  Tick side ≠ 5</t>
+          <t>Price&lt;3,000 Tick side ≠ 1</t>
         </is>
       </c>
       <c r="F41" s="4" t="n">
@@ -3494,7 +3644,7 @@
       </c>
       <c r="I41" s="4" t="inlineStr">
         <is>
-          <t>2282</t>
+          <t>1721</t>
         </is>
       </c>
       <c r="J41" s="4" t="inlineStr">
@@ -3523,7 +3673,7 @@
         </is>
       </c>
       <c r="O41" s="4" t="n">
-        <v>4000.5</v>
+        <v>2500.5</v>
       </c>
       <c r="P41" s="4" t="n"/>
       <c r="Q41" s="4" t="n"/>
@@ -3531,7 +3681,7 @@
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>40</t>
         </is>
       </c>
       <c r="B42" s="4" t="inlineStr">
@@ -3551,7 +3701,7 @@
       </c>
       <c r="E42" s="4" t="inlineStr">
         <is>
-          <t>Price&lt;30,000 Tick side ≠ 10</t>
+          <t>Price&lt;5,000  Tick side ≠ 5</t>
         </is>
       </c>
       <c r="F42" s="4" t="n">
@@ -3569,7 +3719,7 @@
       </c>
       <c r="I42" s="4" t="inlineStr">
         <is>
-          <t>1878</t>
+          <t>2282</t>
         </is>
       </c>
       <c r="J42" s="4" t="inlineStr">
@@ -3598,7 +3748,7 @@
         </is>
       </c>
       <c r="O42" s="4" t="n">
-        <v>15001</v>
+        <v>4000.5</v>
       </c>
       <c r="P42" s="4" t="n"/>
       <c r="Q42" s="4" t="n"/>
@@ -3606,12 +3756,12 @@
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>Quantity Check</t>
+          <t>Tick Size Check</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
@@ -3626,15 +3776,15 @@
       </c>
       <c r="E43" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Quantity=0 </t>
+          <t>Price&lt;30,000 Tick side ≠ 10</t>
         </is>
       </c>
       <c r="F43" s="4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G43" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H43" s="4" t="inlineStr">
@@ -3644,7 +3794,7 @@
       </c>
       <c r="I43" s="4" t="inlineStr">
         <is>
-          <t>1324</t>
+          <t>1878</t>
         </is>
       </c>
       <c r="J43" s="4" t="inlineStr">
@@ -3672,14 +3822,16 @@
           <t>0</t>
         </is>
       </c>
-      <c r="O43" s="4" t="inlineStr"/>
+      <c r="O43" s="4" t="n">
+        <v>15001</v>
+      </c>
       <c r="P43" s="4" t="n"/>
       <c r="Q43" s="4" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>42</t>
         </is>
       </c>
       <c r="B44" s="4" t="inlineStr">
@@ -3699,11 +3851,11 @@
       </c>
       <c r="E44" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Quantity=100(Round-lot) </t>
+          <t xml:space="preserve">Quantity=0 </t>
         </is>
       </c>
       <c r="F44" s="4" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G44" s="4" t="inlineStr">
         <is>
@@ -3752,7 +3904,7 @@
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>43</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
@@ -3772,11 +3924,11 @@
       </c>
       <c r="E45" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Quantity=101(Mixed-lot) </t>
+          <t xml:space="preserve">Quantity=100(Round-lot) </t>
         </is>
       </c>
       <c r="F45" s="4" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G45" s="4" t="inlineStr">
         <is>
@@ -3825,7 +3977,7 @@
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>44</t>
         </is>
       </c>
       <c r="B46" s="4" t="inlineStr">
@@ -3845,11 +3997,11 @@
       </c>
       <c r="E46" s="4" t="inlineStr">
         <is>
-          <t>Quantity=1(Lot size=1)</t>
+          <t xml:space="preserve">Quantity=101(Mixed-lot) </t>
         </is>
       </c>
       <c r="F46" s="4" t="n">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="G46" s="4" t="inlineStr">
         <is>
@@ -3863,7 +4015,7 @@
       </c>
       <c r="I46" s="4" t="inlineStr">
         <is>
-          <t>8421</t>
+          <t>1324</t>
         </is>
       </c>
       <c r="J46" s="4" t="inlineStr">
@@ -3898,7 +4050,7 @@
     <row r="47">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr">
@@ -3918,11 +4070,11 @@
       </c>
       <c r="E47" s="4" t="inlineStr">
         <is>
-          <t>Quantity=10(Lot size=10)</t>
+          <t>Quantity=1(Lot size=1)</t>
         </is>
       </c>
       <c r="F47" s="4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G47" s="4" t="inlineStr">
         <is>
@@ -3936,7 +4088,7 @@
       </c>
       <c r="I47" s="4" t="inlineStr">
         <is>
-          <t>1322</t>
+          <t>8421</t>
         </is>
       </c>
       <c r="J47" s="4" t="inlineStr">
@@ -3971,7 +4123,7 @@
     <row r="48">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B48" s="4" t="inlineStr">
@@ -3995,7 +4147,7 @@
         </is>
       </c>
       <c r="F48" s="4" t="n">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="G48" s="4" t="inlineStr">
         <is>
@@ -4009,7 +4161,7 @@
       </c>
       <c r="I48" s="4" t="inlineStr">
         <is>
-          <t>1773</t>
+          <t>1322</t>
         </is>
       </c>
       <c r="J48" s="4" t="inlineStr">
@@ -4044,12 +4196,12 @@
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>47</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>Order Type Check</t>
+          <t>Quantity Check</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
@@ -4064,15 +4216,15 @@
       </c>
       <c r="E49" s="4" t="inlineStr">
         <is>
-          <t>Order Type is not Limit/Market (Limit/Market Acceptable)</t>
+          <t>Quantity=10(Lot size=10)</t>
         </is>
       </c>
       <c r="F49" s="4" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="G49" s="4" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H49" s="4" t="inlineStr">
@@ -4082,7 +4234,7 @@
       </c>
       <c r="I49" s="4" t="inlineStr">
         <is>
-          <t>1324</t>
+          <t>1773</t>
         </is>
       </c>
       <c r="J49" s="4" t="inlineStr">
@@ -4117,12 +4269,12 @@
     <row r="50">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>48</t>
         </is>
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>TimeInForce Check</t>
+          <t>Order Type Check</t>
         </is>
       </c>
       <c r="C50" s="4" t="inlineStr">
@@ -4137,7 +4289,7 @@
       </c>
       <c r="E50" s="4" t="inlineStr">
         <is>
-          <t>TimeInForce is not 0:Day</t>
+          <t>Order Type is not Limit/Market (Limit/Market Acceptable)</t>
         </is>
       </c>
       <c r="F50" s="4" t="n">
@@ -4145,7 +4297,7 @@
       </c>
       <c r="G50" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H50" s="4" t="inlineStr">
@@ -4160,7 +4312,7 @@
       </c>
       <c r="J50" s="4" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K50" s="4" t="inlineStr">
@@ -4190,12 +4342,12 @@
     <row r="51">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>49</t>
         </is>
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>Order Side Check</t>
+          <t>TimeInForce Check</t>
         </is>
       </c>
       <c r="C51" s="4" t="inlineStr">
@@ -4210,7 +4362,7 @@
       </c>
       <c r="E51" s="4" t="inlineStr">
         <is>
-          <t>Order Side is not Buy/Sell (Buy/Sell Acceptable)</t>
+          <t>TimeInForce is not 0:Day</t>
         </is>
       </c>
       <c r="F51" s="4" t="n">
@@ -4223,7 +4375,7 @@
       </c>
       <c r="H51" s="4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I51" s="4" t="inlineStr">
@@ -4233,7 +4385,7 @@
       </c>
       <c r="J51" s="4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="K51" s="4" t="inlineStr">
@@ -4263,12 +4415,12 @@
     <row r="52">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>50</t>
         </is>
       </c>
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>Account Check</t>
+          <t>Order Side Check</t>
         </is>
       </c>
       <c r="C52" s="4" t="inlineStr">
@@ -4283,7 +4435,7 @@
       </c>
       <c r="E52" s="4" t="inlineStr">
         <is>
-          <t>Account is not the target test account</t>
+          <t>Order Side is not Buy/Sell (Buy/Sell Acceptable)</t>
         </is>
       </c>
       <c r="F52" s="4" t="n">
@@ -4296,7 +4448,7 @@
       </c>
       <c r="H52" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="I52" s="4" t="inlineStr">
@@ -4336,12 +4488,12 @@
     <row r="53">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>51</t>
         </is>
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>Rule80A Check</t>
+          <t>Account Check</t>
         </is>
       </c>
       <c r="C53" s="4" t="inlineStr">
@@ -4356,7 +4508,7 @@
       </c>
       <c r="E53" s="4" t="inlineStr">
         <is>
-          <t>Rule80A is not Agency/Principal</t>
+          <t>Account is not the target test account</t>
         </is>
       </c>
       <c r="F53" s="4" t="n">
@@ -4389,7 +4541,7 @@
       </c>
       <c r="L53" s="4" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>P</t>
         </is>
       </c>
       <c r="M53" s="4" t="inlineStr">
@@ -4409,12 +4561,12 @@
     <row r="54">
       <c r="A54" s="4" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>52</t>
         </is>
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>CashMargin Check</t>
+          <t>Rule80A Check</t>
         </is>
       </c>
       <c r="C54" s="4" t="inlineStr">
@@ -4429,7 +4581,7 @@
       </c>
       <c r="E54" s="4" t="inlineStr">
         <is>
-          <t>CashMargin is not Cash (Cash Acceptable)</t>
+          <t>Rule80A is not Agency/Principal</t>
         </is>
       </c>
       <c r="F54" s="4" t="n">
@@ -4462,12 +4614,12 @@
       </c>
       <c r="L54" s="4" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>S</t>
         </is>
       </c>
       <c r="M54" s="4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="N54" s="4" t="inlineStr">
@@ -4482,12 +4634,12 @@
     <row r="55">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>MarginTransactionType Check</t>
+          <t>CashMargin Check</t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
@@ -4502,7 +4654,7 @@
       </c>
       <c r="E55" s="4" t="inlineStr">
         <is>
-          <t>MarginTransactionType is not 0-None</t>
+          <t>CashMargin is not Cash (Cash Acceptable)</t>
         </is>
       </c>
       <c r="F55" s="4" t="n">
@@ -4540,12 +4692,12 @@
       </c>
       <c r="M55" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="N55" s="4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="O55" s="4" t="inlineStr"/>
@@ -4555,12 +4707,12 @@
     <row r="56">
       <c r="A56" s="4" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>54</t>
         </is>
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>CrossingPriceType Check</t>
+          <t>MarginTransactionType Check</t>
         </is>
       </c>
       <c r="C56" s="4" t="inlineStr">
@@ -4575,7 +4727,7 @@
       </c>
       <c r="E56" s="4" t="inlineStr">
         <is>
-          <t>CrossingPriceType is not ROL/REX</t>
+          <t>MarginTransactionType is not 0-None</t>
         </is>
       </c>
       <c r="F56" s="4" t="n">
@@ -4603,7 +4755,7 @@
       </c>
       <c r="K56" s="4" t="inlineStr">
         <is>
-          <t>ROLX</t>
+          <t>ROL</t>
         </is>
       </c>
       <c r="L56" s="4" t="inlineStr">
@@ -4618,7 +4770,7 @@
       </c>
       <c r="N56" s="4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="O56" s="4" t="inlineStr"/>
@@ -4628,12 +4780,12 @@
     <row r="57">
       <c r="A57" s="4" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>55</t>
         </is>
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>Cancel after Executed</t>
+          <t>CrossingPriceType Check</t>
         </is>
       </c>
       <c r="C57" s="4" t="inlineStr">
@@ -4648,11 +4800,11 @@
       </c>
       <c r="E57" s="4" t="inlineStr">
         <is>
-          <t>New Order-&gt;Canceled</t>
+          <t>CrossingPriceType is not ROL/REX</t>
         </is>
       </c>
       <c r="F57" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G57" s="4" t="inlineStr">
         <is>
@@ -4666,7 +4818,7 @@
       </c>
       <c r="I57" s="4" t="inlineStr">
         <is>
-          <t>6954</t>
+          <t>1324</t>
         </is>
       </c>
       <c r="J57" s="4" t="inlineStr">
@@ -4676,7 +4828,7 @@
       </c>
       <c r="K57" s="4" t="inlineStr">
         <is>
-          <t>ROL</t>
+          <t>ROLX</t>
         </is>
       </c>
       <c r="L57" s="4" t="inlineStr">
@@ -4701,7 +4853,7 @@
     <row r="58">
       <c r="A58" s="4" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="B58" s="4" t="inlineStr">
@@ -4716,7 +4868,7 @@
       </c>
       <c r="D58" s="4" t="inlineStr">
         <is>
-          <t>CancelAck</t>
+          <t>NewAck</t>
         </is>
       </c>
       <c r="E58" s="4" t="inlineStr">
@@ -4739,7 +4891,7 @@
       </c>
       <c r="I58" s="4" t="inlineStr">
         <is>
-          <t>6758</t>
+          <t>6954</t>
         </is>
       </c>
       <c r="J58" s="4" t="inlineStr">
@@ -4774,12 +4926,12 @@
     <row r="59">
       <c r="A59" s="4" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>57</t>
         </is>
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>Absense value for non-required tag</t>
+          <t>Cancel after Executed</t>
         </is>
       </c>
       <c r="C59" s="4" t="inlineStr">
@@ -4789,12 +4941,12 @@
       </c>
       <c r="D59" s="4" t="inlineStr">
         <is>
-          <t>NewAck</t>
+          <t>CancelAck</t>
         </is>
       </c>
       <c r="E59" s="4" t="inlineStr">
         <is>
-          <t>Rule80A</t>
+          <t>New Order-&gt;Canceled</t>
         </is>
       </c>
       <c r="F59" s="4" t="n">
@@ -4812,7 +4964,7 @@
       </c>
       <c r="I59" s="4" t="inlineStr">
         <is>
-          <t>1325</t>
+          <t>6758</t>
         </is>
       </c>
       <c r="J59" s="4" t="inlineStr">
@@ -4825,7 +4977,11 @@
           <t>ROL</t>
         </is>
       </c>
-      <c r="L59" s="4" t="inlineStr"/>
+      <c r="L59" s="4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="M59" s="4" t="inlineStr">
         <is>
           <t>1</t>
@@ -4843,7 +4999,7 @@
     <row r="60">
       <c r="A60" s="4" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>58</t>
         </is>
       </c>
       <c r="B60" s="4" t="inlineStr">
@@ -4863,7 +5019,7 @@
       </c>
       <c r="E60" s="4" t="inlineStr">
         <is>
-          <t>TimeInForce</t>
+          <t>Rule80A</t>
         </is>
       </c>
       <c r="F60" s="4" t="n">
@@ -4884,17 +5040,17 @@
           <t>1325</t>
         </is>
       </c>
-      <c r="J60" s="4" t="inlineStr"/>
+      <c r="J60" s="4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="K60" s="4" t="inlineStr">
         <is>
           <t>ROL</t>
         </is>
       </c>
-      <c r="L60" s="4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
+      <c r="L60" s="4" t="inlineStr"/>
       <c r="M60" s="4" t="inlineStr">
         <is>
           <t>1</t>
@@ -4912,7 +5068,7 @@
     <row r="61">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>59</t>
         </is>
       </c>
       <c r="B61" s="4" t="inlineStr">
@@ -4932,7 +5088,7 @@
       </c>
       <c r="E61" s="4" t="inlineStr">
         <is>
-          <t>CashMargin</t>
+          <t>TimeInForce</t>
         </is>
       </c>
       <c r="F61" s="4" t="n">
@@ -4953,11 +5109,7 @@
           <t>1325</t>
         </is>
       </c>
-      <c r="J61" s="4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="J61" s="4" t="inlineStr"/>
       <c r="K61" s="4" t="inlineStr">
         <is>
           <t>ROL</t>
@@ -4968,7 +5120,11 @@
           <t>P</t>
         </is>
       </c>
-      <c r="M61" s="4" t="inlineStr"/>
+      <c r="M61" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="N61" s="4" t="inlineStr">
         <is>
           <t>0</t>
@@ -4981,7 +5137,7 @@
     <row r="62">
       <c r="A62" s="4" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>60</t>
         </is>
       </c>
       <c r="B62" s="4" t="inlineStr">
@@ -5001,7 +5157,7 @@
       </c>
       <c r="E62" s="4" t="inlineStr">
         <is>
-          <t>CrossingPriceType</t>
+          <t>CashMargin</t>
         </is>
       </c>
       <c r="F62" s="4" t="n">
@@ -5027,17 +5183,17 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K62" s="4" t="inlineStr"/>
+      <c r="K62" s="4" t="inlineStr">
+        <is>
+          <t>ROL</t>
+        </is>
+      </c>
       <c r="L62" s="4" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="M62" s="4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="M62" s="4" t="inlineStr"/>
       <c r="N62" s="4" t="inlineStr">
         <is>
           <t>0</t>
@@ -5050,7 +5206,7 @@
     <row r="63">
       <c r="A63" s="4" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>61</t>
         </is>
       </c>
       <c r="B63" s="4" t="inlineStr">
@@ -5070,7 +5226,7 @@
       </c>
       <c r="E63" s="4" t="inlineStr">
         <is>
-          <t>MarginTransactionType</t>
+          <t>CrossingPriceType</t>
         </is>
       </c>
       <c r="F63" s="4" t="n">
@@ -5096,11 +5252,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K63" s="4" t="inlineStr">
-        <is>
-          <t>ROL</t>
-        </is>
-      </c>
+      <c r="K63" s="4" t="inlineStr"/>
       <c r="L63" s="4" t="inlineStr">
         <is>
           <t>P</t>
@@ -5111,10 +5263,83 @@
           <t>1</t>
         </is>
       </c>
-      <c r="N63" s="4" t="inlineStr"/>
+      <c r="N63" s="4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="O63" s="4" t="inlineStr"/>
       <c r="P63" s="4" t="n"/>
       <c r="Q63" s="4" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="4" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="B64" s="4" t="inlineStr">
+        <is>
+          <t>Absense value for non-required tag</t>
+        </is>
+      </c>
+      <c r="C64" s="4" t="inlineStr">
+        <is>
+          <t>ROLX</t>
+        </is>
+      </c>
+      <c r="D64" s="4" t="inlineStr">
+        <is>
+          <t>NewAck</t>
+        </is>
+      </c>
+      <c r="E64" s="4" t="inlineStr">
+        <is>
+          <t>MarginTransactionType</t>
+        </is>
+      </c>
+      <c r="F64" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G64" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H64" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I64" s="4" t="inlineStr">
+        <is>
+          <t>1325</t>
+        </is>
+      </c>
+      <c r="J64" s="4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K64" s="4" t="inlineStr">
+        <is>
+          <t>ROL</t>
+        </is>
+      </c>
+      <c r="L64" s="4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="M64" s="4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N64" s="4" t="inlineStr"/>
+      <c r="O64" s="4" t="inlineStr"/>
+      <c r="P64" s="4" t="n"/>
+      <c r="Q64" s="4" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>